<commit_message>
Started POM(Page Object Model)
</commit_message>
<xml_diff>
--- a/src/com/metro/testdata/MetroValidLoginTestData.xlsx
+++ b/src/com/metro/testdata/MetroValidLoginTestData.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\Wiley\Selenium\MetroCitySelenium\src\com\metro\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B32A82-8B73-4E57-B8BE-2FDB5492D7D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F4718A-E92E-48AD-B843-C0527E33D429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{A2B653FE-4998-4C4A-95E8-B1D6C0414FB1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginDetails" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>